<commit_message>
Remove some MagmaSat imports that were unnecessary.
</commit_message>
<xml_diff>
--- a/example_data.xlsx
+++ b/example_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiacovin/Dropbox/Research/__Manuscripts in Progress/__ENKI/__TheCode/MagmaSatPlus/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiacovin/Dropbox/Research/__Manuscripts in Progress/__ENKI/__TheCode/VESIcal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA4A9FE-8D58-3F4B-97EC-0991C4824BF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38B49AF-EB7C-0E4C-9169-37ED1E93BC65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="460" windowWidth="27420" windowHeight="17540" xr2:uid="{286DCE04-AB12-484B-880B-42B53AAF1A46}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>SiO2</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>Temp</t>
+  </si>
+  <si>
+    <t>Ma57-3c.3</t>
   </si>
 </sst>
 </file>
@@ -216,7 +219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -225,9 +228,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -551,7 +551,7 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:S15"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -847,7 +847,7 @@
       <c r="P5" s="3">
         <v>4.2149124064868708</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="Q5" s="4">
         <v>4.5659319907785899E-3</v>
       </c>
       <c r="R5">
@@ -906,7 +906,7 @@
       <c r="P6" s="3">
         <v>4.0058157929377556</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="Q6" s="4">
         <v>4.4479634285840598E-3</v>
       </c>
       <c r="R6">
@@ -965,7 +965,7 @@
       <c r="P7" s="3">
         <v>3.8856493407296071</v>
       </c>
-      <c r="Q7" s="5">
+      <c r="Q7" s="4">
         <v>4.6543671039693197E-3</v>
       </c>
       <c r="R7">
@@ -1024,7 +1024,7 @@
       <c r="P8" s="3">
         <v>4.6418428794547735</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="Q8" s="4">
         <v>4.5659319907785899E-3</v>
       </c>
       <c r="R8">
@@ -1083,7 +1083,7 @@
       <c r="P9" s="3">
         <v>4.4021334757226276</v>
       </c>
-      <c r="Q9" s="5">
+      <c r="Q9" s="4">
         <v>4.4479634285840598E-3</v>
       </c>
       <c r="R9">
@@ -1142,7 +1142,7 @@
       <c r="P10" s="3">
         <v>4.2839344334876284</v>
       </c>
-      <c r="Q10" s="5">
+      <c r="Q10" s="4">
         <v>4.5659319907785899E-3</v>
       </c>
       <c r="R10">
@@ -1201,7 +1201,7 @@
       <c r="P11" s="3">
         <v>4.2305325933400617</v>
       </c>
-      <c r="Q11" s="5">
+      <c r="Q11" s="4">
         <v>4.4479634285840598E-3</v>
       </c>
       <c r="R11">
@@ -1260,7 +1260,7 @@
       <c r="P12" s="3">
         <v>4.4597674029594714</v>
       </c>
-      <c r="Q12" s="5">
+      <c r="Q12" s="4">
         <v>4.6543671039693197E-3</v>
       </c>
       <c r="R12">
@@ -1319,7 +1319,7 @@
       <c r="P13" s="3">
         <v>3.7125060458651897</v>
       </c>
-      <c r="Q13" s="5">
+      <c r="Q13" s="4">
         <v>4.4479634285840598E-3</v>
       </c>
       <c r="R13">
@@ -1378,7 +1378,7 @@
       <c r="P14" s="3">
         <v>4.443973024274503</v>
       </c>
-      <c r="Q14" s="5">
+      <c r="Q14" s="4">
         <v>4.6543671039693197E-3</v>
       </c>
       <c r="R14">
@@ -1437,7 +1437,7 @@
       <c r="P15" s="3">
         <v>4.2831710782545924</v>
       </c>
-      <c r="Q15" s="5">
+      <c r="Q15" s="4">
         <v>4.6445226209680503E-3</v>
       </c>
       <c r="R15">
@@ -1447,21 +1447,64 @@
         <v>885</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
+    <row r="16" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="3">
+        <v>77.650000000000006</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.159</v>
+      </c>
+      <c r="D16" s="3">
+        <v>12.28</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0.97689999999999999</v>
+      </c>
+      <c r="H16" s="3">
+        <v>5.9700000000000003E-2</v>
+      </c>
+      <c r="I16" s="3">
+        <v>5.7700000000000001E-2</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0</v>
+      </c>
+      <c r="L16" s="3">
+        <v>0.55979999999999996</v>
+      </c>
+      <c r="M16" s="3">
+        <v>4.08</v>
+      </c>
+      <c r="N16" s="3">
+        <v>4.18</v>
+      </c>
+      <c r="O16" s="3">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="P16" s="3">
+        <v>4.443973024274503</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>4.6543671039693197E-3</v>
+      </c>
+      <c r="R16">
+        <v>100</v>
+      </c>
+      <c r="S16">
+        <v>885</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>